<commit_message>
Updated by Abhishek Birana on 06/10/2023
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="136">
   <si>
     <t>Transport Type</t>
   </si>
@@ -366,6 +366,72 @@
   </si>
   <si>
     <t>AbhishekAutomationSet_141</t>
+  </si>
+  <si>
+    <t>8914089406B9ECDA9ABD560224BA21AA</t>
+  </si>
+  <si>
+    <t>928568EE363B2EBDF512FB34400A7A3F</t>
+  </si>
+  <si>
+    <t>B811134D1A737B32EE3D7D7E74FD25CF</t>
+  </si>
+  <si>
+    <t>08467219D216FA26E95259E738673F9E</t>
+  </si>
+  <si>
+    <t>8A9231F5C8E4CCF3241EA397B1BFC183</t>
+  </si>
+  <si>
+    <t>93859BB0DC05FA7E5511BAC3BDE39929</t>
+  </si>
+  <si>
+    <t>BBDEE7057BEF854034D193D43554FA71</t>
+  </si>
+  <si>
+    <t>95C06C4FF2551BA1A8563DCF2B80BE95</t>
+  </si>
+  <si>
+    <t>F7259D059CDAC1FA3A42A78BFD4F9951</t>
+  </si>
+  <si>
+    <t>74DA6715BF3DE1C34AF4AF5E0AB2D2C8</t>
+  </si>
+  <si>
+    <t>1D3DD0B20CED73FB873175573F8726F9</t>
+  </si>
+  <si>
+    <t>FE763F8A63493EEDB1667320D04C3847</t>
+  </si>
+  <si>
+    <t>12B6926FE41D54B18A6AC80B396C3226</t>
+  </si>
+  <si>
+    <t>0D01B6F921D36F3F5B0168C6A9D1A55C</t>
+  </si>
+  <si>
+    <t>9853C2EB9086D95F3614627B1D750231</t>
+  </si>
+  <si>
+    <t>479A9C09BA901C979953C50FF6A917CA</t>
+  </si>
+  <si>
+    <t>E36D3E00708C26E7B0A446B40BC6F2FD</t>
+  </si>
+  <si>
+    <t>E73DBDE11D43C5110582FBAF08173406</t>
+  </si>
+  <si>
+    <t>CD55C752FAD822BC6F7C9B97B29738E6</t>
+  </si>
+  <si>
+    <t>D84874FBA1D04A938BBB0A100B6E7BB5</t>
+  </si>
+  <si>
+    <t>AbhishekAutomationProfile722</t>
+  </si>
+  <si>
+    <t>AbhishekAutomationSet_263</t>
   </si>
 </sst>
 </file>
@@ -819,7 +885,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>113</v>
+        <v>135</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>11</v>
@@ -891,7 +957,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>111</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -932,7 +998,7 @@
     </row>
     <row r="2" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
-        <v>112</v>
+        <v>134</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>84</v>

</xml_diff>

<commit_message>
Updated by Abhishek Birana on 09/10/2023
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData.xlsx
+++ b/src/test/resources/TestData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="172">
   <si>
     <t>Transport Type</t>
   </si>
@@ -504,6 +504,42 @@
   </si>
   <si>
     <t>AbhishekAutomationSet_446</t>
+  </si>
+  <si>
+    <t>10B4C9373E4E38256C24BBAE3C9A8C7A</t>
+  </si>
+  <si>
+    <t>AbhishekAutomationProfile492</t>
+  </si>
+  <si>
+    <t>AbhishekAutomationSet_289</t>
+  </si>
+  <si>
+    <t>66420720313AC5A832922E2860F9938E</t>
+  </si>
+  <si>
+    <t>AbhishekAutomationProfile736</t>
+  </si>
+  <si>
+    <t>AbhishekAutomationSet_799</t>
+  </si>
+  <si>
+    <t>FFEFE07CC8D8D603163C35D83DAA9CB0</t>
+  </si>
+  <si>
+    <t>AbhishekAutomationProfile629</t>
+  </si>
+  <si>
+    <t>AbhishekAutomationSet_848</t>
+  </si>
+  <si>
+    <t>9E5127EE52738795DF4184CE0AFA797A</t>
+  </si>
+  <si>
+    <t>AbhishekAutomationProfile125</t>
+  </si>
+  <si>
+    <t>AbhishekAutomationSet_164</t>
   </si>
 </sst>
 </file>
@@ -957,7 +993,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>11</v>
@@ -1029,7 +1065,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
     </row>
   </sheetData>
@@ -1070,7 +1106,7 @@
     </row>
     <row r="2" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
-        <v>158</v>
+        <v>170</v>
       </c>
       <c r="B2" s="9" t="s">
         <v>84</v>

</xml_diff>